<commit_message>
updated all individual and average plots to include R* runs
</commit_message>
<xml_diff>
--- a/main/RunSchdule.xlsx
+++ b/main/RunSchdule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21720" yWindow="3760" windowWidth="26880" windowHeight="26740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37740" windowHeight="24260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -267,11 +267,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -341,7 +359,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="64">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -365,6 +383,15 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -387,6 +414,15 @@
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -718,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="U40" sqref="U40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1205,7 +1241,7 @@
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
-      <c r="H28" s="21"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
@@ -1553,7 +1589,7 @@
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
-      <c r="H50" s="23"/>
+      <c r="H50" s="21"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
@@ -1571,7 +1607,7 @@
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
-      <c r="H51" s="23"/>
+      <c r="H51" s="21"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
@@ -1607,7 +1643,7 @@
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
-      <c r="H53" s="23"/>
+      <c r="H53" s="21"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
@@ -1625,7 +1661,7 @@
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
-      <c r="H54" s="23"/>
+      <c r="H54" s="21"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
@@ -1643,7 +1679,7 @@
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
-      <c r="H55" s="23"/>
+      <c r="H55" s="21"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
@@ -1661,7 +1697,7 @@
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
-      <c r="H56" s="23"/>
+      <c r="H56" s="21"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
@@ -1679,7 +1715,7 @@
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
-      <c r="H57" s="23"/>
+      <c r="H57" s="21"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
@@ -1697,7 +1733,7 @@
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
-      <c r="H58" s="23"/>
+      <c r="H58" s="21"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
@@ -1715,7 +1751,7 @@
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
-      <c r="H59" s="23"/>
+      <c r="H59" s="20"/>
       <c r="I59" s="11"/>
       <c r="J59" s="11"/>
       <c r="K59" s="11"/>
@@ -1798,7 +1834,7 @@
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
-      <c r="H65" s="23"/>
+      <c r="H65" s="14"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
@@ -1816,7 +1852,7 @@
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
-      <c r="H66" s="23"/>
+      <c r="H66" s="14"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
@@ -1829,16 +1865,16 @@
       <c r="B67" s="7">
         <v>5</v>
       </c>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
-      <c r="H67" s="23"/>
-      <c r="I67" s="23"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="23"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
       <c r="M67" s="23"/>
       <c r="N67" s="23"/>
       <c r="O67" s="23"/>
@@ -1852,7 +1888,7 @@
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
-      <c r="H68" s="23"/>
+      <c r="H68" s="14"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
@@ -1870,7 +1906,7 @@
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
-      <c r="H69" s="23"/>
+      <c r="H69" s="14"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
@@ -1888,7 +1924,7 @@
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
-      <c r="H70" s="23"/>
+      <c r="H70" s="14"/>
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
@@ -1906,7 +1942,7 @@
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
-      <c r="H71" s="23"/>
+      <c r="H71" s="14"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
@@ -1924,7 +1960,7 @@
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
-      <c r="H72" s="23"/>
+      <c r="H72" s="14"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
@@ -1942,7 +1978,7 @@
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
-      <c r="H73" s="23"/>
+      <c r="H73" s="14"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
@@ -1960,7 +1996,7 @@
       <c r="E74" s="11"/>
       <c r="F74" s="11"/>
       <c r="G74" s="11"/>
-      <c r="H74" s="23"/>
+      <c r="H74" s="20"/>
       <c r="I74" s="11"/>
       <c r="J74" s="11"/>
       <c r="K74" s="11"/>

</xml_diff>